<commit_message>
Built out physical ports and beging L3 out config
</commit_message>
<xml_diff>
--- a/acibootstrap/files/vars/acibootstrap.xlsx
+++ b/acibootstrap/files/vars/acibootstrap.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8160" windowWidth="24020" windowHeight="15840" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="8160" windowWidth="24020" windowHeight="15840" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="fabric_pol" sheetId="1" r:id="rId1"/>
     <sheet name="mgmt" sheetId="5" r:id="rId2"/>
     <sheet name="vcenter" sheetId="4" r:id="rId3"/>
-    <sheet name="poc_tenant" sheetId="2" r:id="rId4"/>
-    <sheet name="menu items" sheetId="3" r:id="rId5"/>
+    <sheet name="phys port map" sheetId="6" r:id="rId4"/>
+    <sheet name="poc_tenant" sheetId="2" r:id="rId5"/>
+    <sheet name="menu items" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="88">
   <si>
     <t>n300_America-Chicago</t>
   </si>
@@ -195,9 +196,6 @@
     <t>Static</t>
   </si>
   <si>
-    <t>BGP</t>
-  </si>
-  <si>
     <t>OSPF</t>
   </si>
   <si>
@@ -226,6 +224,78 @@
   </si>
   <si>
     <t>administrator@vsphere.local</t>
+  </si>
+  <si>
+    <t>Device Type</t>
+  </si>
+  <si>
+    <t>Rack Server</t>
+  </si>
+  <si>
+    <t>l2_out_switch_speed</t>
+  </si>
+  <si>
+    <t>Routed Out</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>Protocols</t>
+  </si>
+  <si>
+    <t>OSFP</t>
+  </si>
+  <si>
+    <t>ospf_area_id</t>
+  </si>
+  <si>
+    <t>ospf_area_type</t>
+  </si>
+  <si>
+    <t>OSFP Area Types</t>
+  </si>
+  <si>
+    <t>nssa</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>stub</t>
+  </si>
+  <si>
+    <t>Leaf 101 router id</t>
+  </si>
+  <si>
+    <t>Leaf 102 router id</t>
+  </si>
+  <si>
+    <t>1.102.1.2</t>
+  </si>
+  <si>
+    <t>1.101.1.2</t>
+  </si>
+  <si>
+    <t>Leaf 101 routed Address</t>
+  </si>
+  <si>
+    <t>10.10.10.1/30</t>
+  </si>
+  <si>
+    <t>Leaf 102 routed Address</t>
+  </si>
+  <si>
+    <t>10.10.11.1/30</t>
+  </si>
+  <si>
+    <t>Routed External Vlans</t>
+  </si>
+  <si>
+    <t>VLAN Encap</t>
+  </si>
+  <si>
+    <t>0.0.0.2</t>
   </si>
 </sst>
 </file>
@@ -523,13 +593,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -566,9 +637,10 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -847,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -936,6 +1008,14 @@
         <v>48</v>
       </c>
       <c r="B10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
         <v>51</v>
       </c>
     </row>
@@ -960,7 +1040,7 @@
           <x14:formula1>
             <xm:f>'menu items'!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B10</xm:sqref>
+          <xm:sqref>B10 B11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -987,27 +1067,27 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="17"/>
       <c r="B2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1043,7 +1123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1100,7 +1180,7 @@
         <v>42</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1125,15 +1205,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1208,16 +1300,117 @@
         <v>27</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'menu items'!$B$2:$B$3</xm:f>
           </x14:formula1>
           <xm:sqref>B7:B10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'menu items'!$E$2:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'menu items'!$H$2:$H$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'menu items'!$I$2:$I$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>B18 B23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1225,21 +1418,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1255,8 +1450,20 @@
       <c r="E1" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -1272,8 +1479,20 @@
       <c r="E2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1284,10 +1503,19 @@
         <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3">
+        <v>2111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -1295,15 +1523,51 @@
         <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
-        <v>56</v>
+      <c r="I5">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>2119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ospf, eigrp, and static routing for POC tenant complete
</commit_message>
<xml_diff>
--- a/acibootstrap/files/vars/acibootstrap.xlsx
+++ b/acibootstrap/files/vars/acibootstrap.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8160" windowWidth="24020" windowHeight="15840" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="5760" windowWidth="24020" windowHeight="15840" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="fabric_pol" sheetId="1" r:id="rId1"/>
     <sheet name="mgmt" sheetId="5" r:id="rId2"/>
     <sheet name="vcenter" sheetId="4" r:id="rId3"/>
-    <sheet name="phys port map" sheetId="6" r:id="rId4"/>
-    <sheet name="poc_tenant" sheetId="2" r:id="rId5"/>
+    <sheet name="poc_tenant" sheetId="2" r:id="rId4"/>
+    <sheet name="phys port map" sheetId="6" r:id="rId5"/>
     <sheet name="menu items" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
   <si>
     <t>n300_America-Chicago</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>POC-3tier</t>
-  </si>
-  <si>
     <t>bgp_as</t>
   </si>
   <si>
@@ -296,6 +293,30 @@
   </si>
   <si>
     <t>0.0.0.2</t>
+  </si>
+  <si>
+    <t>POC-3tier-L3</t>
+  </si>
+  <si>
+    <t>eigrp_as</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
+    <t>Next-Hop</t>
+  </si>
+  <si>
+    <t>0.0.0.0/0</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>10.10.10.2</t>
+  </si>
+  <si>
+    <t>10.10.11.2</t>
   </si>
 </sst>
 </file>
@@ -354,7 +375,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -456,32 +477,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -514,15 +509,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -550,43 +536,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -602,7 +551,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -617,19 +566,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -922,7 +867,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -941,39 +886,39 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -981,7 +926,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -989,7 +934,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>3</v>
@@ -997,7 +942,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -1005,18 +950,18 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1050,10 +995,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D10"/>
+  <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1064,55 +1009,94 @@
     <col min="4" max="4" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="15"/>
+      <c r="B2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="16" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1133,17 +1117,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="24"/>
+      <c r="A1" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1156,39 +1140,39 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
         <v>45</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
         <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1205,22 +1189,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1238,7 +1210,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1255,7 +1227,7 @@
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>$B$2</f>
-        <v>POC-3tier</v>
+        <v>POC-3tier-L3</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -1267,7 +1239,7 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f t="shared" ref="A8:A10" si="0">$B$2</f>
-        <v>POC-3tier</v>
+        <v>POC-3tier-L3</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -1279,7 +1251,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>POC-3tier</v>
+        <v>POC-3tier-L3</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -1291,47 +1263,47 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>POC-3tier</v>
+        <v>POC-3tier-L3</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
         <v>81</v>
-      </c>
-      <c r="B17" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B18">
         <v>2110</v>
@@ -1339,23 +1311,23 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
         <v>78</v>
-      </c>
-      <c r="B21" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s">
         <v>83</v>
-      </c>
-      <c r="B22" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B23">
         <v>2110</v>
@@ -1363,23 +1335,75 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>102</v>
+      </c>
+      <c r="B37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1418,6 +1442,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
@@ -1442,51 +1478,51 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
         <v>53</v>
       </c>
-      <c r="F2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" t="s">
-        <v>54</v>
-      </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I2">
         <v>2110</v>
@@ -1500,16 +1536,16 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I3">
         <v>2111</v>
@@ -1517,16 +1553,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I4">
         <v>2112</v>
@@ -1534,7 +1570,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5">
         <v>2113</v>

</xml_diff>

<commit_message>
import new data format
</commit_message>
<xml_diff>
--- a/acibootstrap/files/vars/acibootstrap.xlsx
+++ b/acibootstrap/files/vars/acibootstrap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5760" windowWidth="24020" windowHeight="15840" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="5760" windowWidth="24020" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="fabric_pol" sheetId="1" r:id="rId1"/>
@@ -866,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1191,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>